<commit_message>
Adding UoW Category to configuration spreadsheets and initialization ETL
git-svn-id: svn://svn-staging.maximus.com/dev1d/maxdat@12073 3a208796-2f9a-46b6-afea-cdc47f3b9e6b
</commit_message>
<xml_diff>
--- a/ContactCenter/trunk/kettle/MAXDAT/implementation/BOS/data/configuration.xlsx
+++ b/ContactCenter/trunk/kettle/MAXDAT/implementation/BOS/data/configuration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="240" windowWidth="11280" windowHeight="7725" tabRatio="762"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="11280" windowHeight="7725" tabRatio="762" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
@@ -305,7 +305,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="456">
   <si>
     <t>PROJECT_NAME</t>
   </si>
@@ -1664,6 +1664,15 @@
   </si>
   <si>
     <t>Staff Group ID</t>
+  </si>
+  <si>
+    <t>unit_of_work_category</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>INBOUND_CALL</t>
   </si>
 </sst>
 </file>
@@ -2156,8 +2165,8 @@
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10007,10 +10016,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10019,9 +10028,10 @@
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>231</v>
       </c>
@@ -10037,8 +10047,11 @@
       <c r="E1" s="11" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="28">
         <v>0</v>
       </c>
@@ -10054,8 +10067,11 @@
       <c r="E2" s="28" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="28">
         <v>1</v>
       </c>
@@ -10071,8 +10087,11 @@
       <c r="E3" s="28" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="28">
         <v>2</v>
       </c>
@@ -10088,8 +10107,11 @@
       <c r="E4" s="28" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="28">
         <v>3</v>
       </c>
@@ -10105,8 +10127,11 @@
       <c r="E5" s="28" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="28">
         <v>4</v>
       </c>
@@ -10122,8 +10147,11 @@
       <c r="E6" s="28" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="28">
         <v>5</v>
       </c>
@@ -10139,8 +10167,11 @@
       <c r="E7" s="28" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="28" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="28">
         <v>6</v>
       </c>
@@ -10156,8 +10187,11 @@
       <c r="E8" s="28" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="28" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="28">
         <v>7</v>
       </c>
@@ -10172,6 +10206,9 @@
       </c>
       <c r="E9" s="28" t="s">
         <v>237</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>455</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding/Updating files related to addition of INCLUDE_IN_REPORTS_FLAG to CC_D_PROJECT and CC_D_PROGRAM tables
git-svn-id: svn://svn-staging.maximus.com/dev1d/maxdat@12075 3a208796-2f9a-46b6-afea-cdc47f3b9e6b
</commit_message>
<xml_diff>
--- a/ContactCenter/trunk/kettle/MAXDAT/implementation/BOS/data/configuration.xlsx
+++ b/ContactCenter/trunk/kettle/MAXDAT/implementation/BOS/data/configuration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="240" windowWidth="11280" windowHeight="7725" tabRatio="762" activeTab="8"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="11280" windowHeight="7725" tabRatio="762"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="1" r:id="rId1"/>
@@ -305,7 +305,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1467" uniqueCount="457">
   <si>
     <t>PROJECT_NAME</t>
   </si>
@@ -1673,6 +1673,9 @@
   </si>
   <si>
     <t>INBOUND_CALL</t>
+  </si>
+  <si>
+    <t>INCLUDE_IN_REPORTS_FLAG</t>
   </si>
 </sst>
 </file>
@@ -2163,10 +2166,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2182,9 +2185,10 @@
     <col min="9" max="9" width="12.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>229</v>
       </c>
@@ -2218,8 +2222,11 @@
       <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -2252,6 +2259,9 @@
       </c>
       <c r="K2" s="16">
         <v>401768</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -10018,8 +10028,8 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>